<commit_message>
Format config and add unit columns to Excel input file for tests
</commit_message>
<xml_diff>
--- a/message_ix/tests/data/westeros_macro_input.xlsx
+++ b/message_ix/tests/data/westeros_macro_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wienpahl\Desktop\PythonProjects\LauWien\message_ix\message_ix\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakeri\Documents\Github\message_ix\message_ix\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A948E7-73F5-45EE-A988-C68D3FF53310}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE44DA44-539A-4418-80D6-1165D2CDF36A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9210" yWindow="1185" windowWidth="17355" windowHeight="11955" tabRatio="979" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="12270" tabRatio="979" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="price_ref" sheetId="1" r:id="rId1"/>
@@ -32,10 +32,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -46,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="21">
   <si>
     <t>node</t>
   </si>
@@ -66,6 +63,15 @@
     <t>light</t>
   </si>
   <si>
+    <t>15 more than value in first period</t>
+  </si>
+  <si>
+    <t>reduced from value found in COST_NODAL_NET</t>
+  </si>
+  <si>
+    <t>10 less than first period</t>
+  </si>
+  <si>
     <t>taken from existing macro data files</t>
   </si>
   <si>
@@ -78,25 +84,28 @@
     <t>just made up, but taken from existing macro data files</t>
   </si>
   <si>
-    <t>ignore_nodes</t>
-  </si>
-  <si>
-    <t>ignore_sectors</t>
-  </si>
-  <si>
-    <t>foo</t>
-  </si>
-  <si>
-    <t>bar</t>
-  </si>
-  <si>
-    <t>rounded value, demand_per_year * 0.5</t>
-  </si>
-  <si>
-    <t>reduced by same factor than before's cost_ref value ( 0.01747775 (year 700) - 0.015 (year 690)  = 0.00247775; value 15 was found in COST_NODAL_NET</t>
-  </si>
-  <si>
-    <t>300 less than value in first period</t>
+    <t>level</t>
+  </si>
+  <si>
+    <t>useful</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>USD/kWa</t>
+  </si>
+  <si>
+    <t>G$</t>
+  </si>
+  <si>
+    <t>GWa</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>T$</t>
   </si>
 </sst>
 </file>
@@ -132,10 +141,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,166 +461,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.42578125"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1">
-        <f>511-300</f>
-        <v>211</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1025" width="8.42578125"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <v>680</v>
-      </c>
-      <c r="C2" s="1">
-        <v>350</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>690</v>
-      </c>
-      <c r="C3" s="1">
-        <v>500</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>700</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>710</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2000</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>720</v>
-      </c>
-      <c r="C6" s="1">
-        <v>3000</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1025" width="8.42578125"/>
+    <col min="1" max="3" width="8.42578125"/>
+    <col min="5" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -617,13 +478,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -633,67 +494,16 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1">
-        <v>690</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2">
-        <v>0.02</v>
+      <c r="C2" s="1">
+        <v>195</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>700</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>710</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>720</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -703,73 +513,120 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:D4"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.42578125"/>
+    <col min="1" max="3" width="8.42578125"/>
+    <col min="5" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
+        <v>680</v>
+      </c>
+      <c r="C2" s="1">
+        <v>350</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>690</v>
+      </c>
+      <c r="C3" s="1">
+        <v>500</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
         <v>700</v>
       </c>
-      <c r="C2" s="1">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="C4" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
         <v>710</v>
       </c>
-      <c r="C3" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="C5" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
         <v>720</v>
       </c>
-      <c r="C4" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
+      <c r="C6" s="1">
+        <v>3000</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -778,12 +635,220 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="8.42578125"/>
+    <col min="6" max="1026" width="8.42578125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>690</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>700</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>710</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>720</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="8.42578125"/>
+    <col min="5" max="1026" width="8.42578125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>700</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>710</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>720</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,20 +856,26 @@
     <col min="1" max="1025" width="11.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -819,57 +890,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.42578125"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <f>9.17583/1000</f>
-        <v>9.1758299999999994E-3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1025" width="8.42578125"/>
+    <col min="1" max="2" width="8.42578125"/>
+    <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -877,10 +907,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -890,14 +920,15 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1">
-        <v>27</v>
+      <c r="B2" s="1">
+        <f>15/1000</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -906,39 +937,52 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C2"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.42578125"/>
+    <col min="1" max="3" width="8.42578125"/>
+    <col min="5" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>90</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -947,20 +991,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C2"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.42578125"/>
+    <col min="1" max="2" width="8.42578125"/>
+    <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -968,18 +1013,24 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>0.05</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -988,20 +1039,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C2"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.42578125"/>
+    <col min="1" max="2" width="8.42578125"/>
+    <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1009,18 +1061,24 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>0.2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1029,20 +1087,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C2"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.42578125"/>
+    <col min="1" max="2" width="8.42578125"/>
+    <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1050,18 +1109,24 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>0.05</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1070,20 +1135,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C2"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.42578125"/>
+    <col min="1" max="2" width="8.42578125"/>
+    <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1091,18 +1157,24 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>0.05</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1111,20 +1183,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C2"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.42578125"/>
+    <col min="1" max="2" width="8.42578125"/>
+    <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1132,18 +1205,72 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="8.42578125"/>
+    <col min="4" max="1026" width="8.42578125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update input data based on the latest xls file
</commit_message>
<xml_diff>
--- a/message_ix/tests/data/westeros_macro_input.xlsx
+++ b/message_ix/tests/data/westeros_macro_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakeri\Documents\Github\message_ix\message_ix\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695EA837-2C13-4885-86C7-5501E8F0242A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{32427D37-8FED-4FEC-82F2-D3F690308589}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="345" windowWidth="21600" windowHeight="12360" tabRatio="979" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17025" yWindow="3105" windowWidth="13425" windowHeight="10875" tabRatio="979" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="price_ref" sheetId="1" r:id="rId1"/>
@@ -66,15 +66,6 @@
     <t>light</t>
   </si>
   <si>
-    <t>15 more than value in first period</t>
-  </si>
-  <si>
-    <t>reduced from value found in COST_NODAL_NET</t>
-  </si>
-  <si>
-    <t>10 less than first period</t>
-  </si>
-  <si>
     <t>taken from existing macro data files</t>
   </si>
   <si>
@@ -87,31 +78,40 @@
     <t>just made up, but taken from existing macro data files</t>
   </si>
   <si>
+    <t>rounded value, demand_per_year * 0.5</t>
+  </si>
+  <si>
+    <t>reduced by same factor than before's cost_ref value ( 0.01747775 (year 700) - 0.015 (year 690)  = 0.00247775; value 15 was found in COST_NODAL_NET</t>
+  </si>
+  <si>
+    <t>300 less than value in first period</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>USD/kWa</t>
+  </si>
+  <si>
+    <t>G$</t>
+  </si>
+  <si>
+    <t>GWa</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>T$</t>
+  </si>
+  <si>
+    <t>commodity</t>
+  </si>
+  <si>
     <t>level</t>
   </si>
   <si>
     <t>useful</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>USD/kWa</t>
-  </si>
-  <si>
-    <t>G$</t>
-  </si>
-  <si>
-    <t>GWa</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>T$</t>
-  </si>
-  <si>
-    <t>commodity</t>
   </si>
 </sst>
 </file>
@@ -147,12 +147,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,7 +471,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,7 +491,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -504,18 +505,19 @@
         <v>5</v>
       </c>
       <c r="C2" s="1">
-        <v>195</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
+        <f>511-300</f>
+        <v>211</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -523,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,13 +540,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -560,11 +562,11 @@
       <c r="C2" s="1">
         <v>350</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
+      <c r="D2" t="s">
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -577,11 +579,11 @@
       <c r="C3" s="1">
         <v>500</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
+      <c r="D3" t="s">
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -594,11 +596,11 @@
       <c r="C4" s="1">
         <v>1000</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>20</v>
+      <c r="D4" t="s">
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -611,11 +613,11 @@
       <c r="C5" s="1">
         <v>2000</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
+      <c r="D5" t="s">
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -628,28 +630,28 @@
       <c r="C6" s="1">
         <v>3000</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
+      <c r="D6" t="s">
+        <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
         <v>730</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>3000</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>11</v>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -663,7 +665,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +679,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -686,7 +688,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -702,14 +704,14 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <v>0.02</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>19</v>
+      <c r="E2" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -722,14 +724,14 @@
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <v>0.02</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>19</v>
+      <c r="E3" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -742,14 +744,14 @@
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="2">
         <v>0.02</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>19</v>
+      <c r="E4" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -762,14 +764,14 @@
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <v>0.02</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>19</v>
+      <c r="E5" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -783,7 +785,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,13 +799,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -819,11 +821,11 @@
       <c r="C2" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
+      <c r="D2" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -836,11 +838,11 @@
       <c r="C3" s="1">
         <v>1.8</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
+      <c r="D3" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -853,11 +855,11 @@
       <c r="C4" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>19</v>
+      <c r="D4" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -870,15 +872,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.28515625"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="1026" width="11.28515625"/>
+    <col min="1" max="1025" width="11.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -889,13 +889,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -909,19 +909,19 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="1">
+        <v>21</v>
+      </c>
+      <c r="E2">
         <v>700</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E3" s="1">
+      <c r="E3">
         <v>710</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E4" s="1">
+      <c r="E4">
         <v>720</v>
       </c>
     </row>
@@ -937,6 +937,157 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="8.42578125"/>
+    <col min="4" max="1026" width="8.42578125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <f>9.17583/1000</f>
+        <v>9.1758299999999994E-3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="8.42578125"/>
+    <col min="5" max="1026" width="8.42578125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="8.42578125"/>
+    <col min="4" max="1026" width="8.42578125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -957,7 +1108,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -968,14 +1119,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <f>15/1000</f>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="C2" s="1" t="s">
+        <v>0.2</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -984,66 +1134,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="3" width="8.42578125"/>
-    <col min="5" max="1026" width="8.42578125"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1">
-        <v>90</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,7 +1156,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1073,11 +1169,11 @@
       <c r="B2" s="1">
         <v>0.05</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>19</v>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1086,200 +1182,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="8.42578125"/>
-    <col min="4" max="1026" width="8.42578125"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="8.42578125"/>
-    <col min="4" max="1026" width="8.42578125"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="8.42578125"/>
-    <col min="4" max="1026" width="8.42578125"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="8.42578125"/>
-    <col min="4" max="1026" width="8.42578125"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1300,7 +1204,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1311,13 +1215,109 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="8.42578125"/>
+    <col min="4" max="1026" width="8.42578125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>19</v>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="8.42578125"/>
+    <col min="4" max="1026" width="8.42578125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjust xlsx after rebase
</commit_message>
<xml_diff>
--- a/message_ix/tests/data/westeros_macro_input.xlsx
+++ b/message_ix/tests/data/westeros_macro_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakeri\Documents\Github\message_ix\message_ix\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura\ProgrammingProjects\LauWien\message_ix\message_ix\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32427D37-8FED-4FEC-82F2-D3F690308589}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3C48BD-8129-4F81-AECC-783B6BBDF77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17025" yWindow="3105" windowWidth="13425" windowHeight="10875" tabRatio="979" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1560" windowWidth="17745" windowHeight="12945" tabRatio="979" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="price_ref" sheetId="1" r:id="rId1"/>
@@ -156,7 +156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -172,7 +172,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -474,7 +474,7 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="8.42578125"/>
     <col min="5" max="1026" width="8.42578125"/>
@@ -529,7 +529,7 @@
       <selection activeCell="A7" sqref="A7:J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="8.42578125"/>
     <col min="5" max="1026" width="8.42578125"/>
@@ -668,7 +668,7 @@
       <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="8.42578125"/>
     <col min="6" max="1026" width="8.42578125"/>
@@ -788,7 +788,7 @@
       <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="8.42578125"/>
     <col min="5" max="1026" width="8.42578125"/>
@@ -872,11 +872,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1025" width="11.28515625"/>
   </cols>
@@ -939,11 +939,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
@@ -968,8 +968,8 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <f>9.17583/1000</f>
-        <v>9.1758299999999994E-3</v>
+        <f>0.00866017-0.00247775</f>
+        <v>6.1824200000000001E-3</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -992,7 +992,7 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="8.42578125"/>
     <col min="5" max="1026" width="8.42578125"/>
@@ -1046,7 +1046,7 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
@@ -1094,7 +1094,7 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
@@ -1142,7 +1142,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
@@ -1190,7 +1190,7 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
@@ -1238,7 +1238,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
@@ -1286,7 +1286,7 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>

</xml_diff>

<commit_message>
Adjust macro related tests to account for changes
</commit_message>
<xml_diff>
--- a/message_ix/tests/data/westeros_macro_input.xlsx
+++ b/message_ix/tests/data/westeros_macro_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura\ProgrammingProjects\LauWien\message_ix\message_ix\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\message_ix\message_ix\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3C48BD-8129-4F81-AECC-783B6BBDF77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78FFAA4-120F-464E-8003-FFB11A403A74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1560" windowWidth="17745" windowHeight="12945" tabRatio="979" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="979" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="price_ref" sheetId="1" r:id="rId1"/>
@@ -147,16 +147,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -172,7 +170,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -474,44 +472,44 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="8.42578125"/>
     <col min="5" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <f>511-300</f>
         <v>211</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -529,111 +527,111 @@
       <selection activeCell="A7" sqref="A7:J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="8.42578125"/>
     <col min="5" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>680</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>350</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
         <v>690</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>500</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
         <v>700</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>1000</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>710</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>2000</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <v>720</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>3000</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -668,109 +666,109 @@
       <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="8.42578125"/>
     <col min="6" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>690</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>0.02</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
         <v>700</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>0.02</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
         <v>710</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>0.02</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>720</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>0.02</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -788,77 +786,77 @@
       <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="8.42578125"/>
     <col min="5" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>700</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
         <v>710</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>1.8</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
         <v>720</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -876,7 +874,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1025" width="11.28515625"/>
   </cols>
@@ -943,38 +941,38 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <f>0.00866017-0.00247775</f>
-        <v>6.1824200000000001E-3</v>
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <f>(0.00866017-0.00247775)*1000</f>
+        <v>6.1824200000000005</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -992,43 +990,43 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="8.42578125"/>
     <col min="5" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>27</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1046,37 +1044,37 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>0.05</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1094,37 +1092,37 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>0.2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1142,37 +1140,37 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>0.05</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1190,37 +1188,37 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>0.05</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1238,37 +1236,37 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>0.3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1286,37 +1284,37 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correct calculation of COST_NODAL_NET for standalone MESSAGE (#648)
* Correct calculation of COST_NODAL_NET for standalone MESSAGE

* Adjust macro related tests to account for changes

* Extend documentation on macro calibration process

* Update release notes for PR#648

* Add intersphinx_mapping for message_doc

* Extend references

* Extend description of MESSAGE-MACRO calibration process/needs

* Enhance the readability of calibration process

Co-authored-by: Behnam Zakeri <30926636+behnam-zakeri@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/message_ix/tests/data/westeros_macro_input.xlsx
+++ b/message_ix/tests/data/westeros_macro_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura\ProgrammingProjects\LauWien\message_ix\message_ix\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\message_ix\message_ix\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3C48BD-8129-4F81-AECC-783B6BBDF77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78FFAA4-120F-464E-8003-FFB11A403A74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1560" windowWidth="17745" windowHeight="12945" tabRatio="979" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="979" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="price_ref" sheetId="1" r:id="rId1"/>
@@ -147,16 +147,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -172,7 +170,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -474,44 +472,44 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="8.42578125"/>
     <col min="5" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <f>511-300</f>
         <v>211</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -529,111 +527,111 @@
       <selection activeCell="A7" sqref="A7:J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="8.42578125"/>
     <col min="5" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>680</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>350</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
         <v>690</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>500</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
         <v>700</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>1000</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>710</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>2000</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <v>720</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>3000</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -668,109 +666,109 @@
       <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="8.42578125"/>
     <col min="6" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>690</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>0.02</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
         <v>700</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>0.02</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
         <v>710</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>0.02</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>720</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>0.02</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -788,77 +786,77 @@
       <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="8.42578125"/>
     <col min="5" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>700</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
         <v>710</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>1.8</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
         <v>720</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -876,7 +874,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1025" width="11.28515625"/>
   </cols>
@@ -943,38 +941,38 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <f>0.00866017-0.00247775</f>
-        <v>6.1824200000000001E-3</v>
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <f>(0.00866017-0.00247775)*1000</f>
+        <v>6.1824200000000005</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -992,43 +990,43 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="8.42578125"/>
     <col min="5" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>27</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1046,37 +1044,37 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>0.05</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1094,37 +1092,37 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>0.2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1142,37 +1140,37 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>0.05</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1190,37 +1188,37 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>0.05</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1238,37 +1236,37 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>0.3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1286,37 +1284,37 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125"/>
     <col min="4" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>